<commit_message>
#42 npcshop support differenet types of resource cost
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/NpcShop.xlsx
+++ b/ConfigData/Xlsx/NpcShop.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassic\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="NpcShop" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -48,9 +48,6 @@
     <t>10501;2|20501;2|30501;2|40501;2|50501;2</t>
   </si>
   <si>
-    <t>33001;1|33002;1|33010;1|20004;1</t>
-  </si>
-  <si>
     <t>10101;1|10102;1</t>
   </si>
   <si>
@@ -61,6 +58,22 @@
   </si>
   <si>
     <t>11501;2|21501;2|31501;2|41501;2|51501;2</t>
+  </si>
+  <si>
+    <t>MoneyType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>货币类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>22031002;1|22031003;1|22031004;1|22031005;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -747,11 +760,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="SellTable"/>
+    <tableColumn id="3" name="MoneyType"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1044,103 +1058,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>44000001</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>44000002</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>44010001</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>44010003</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>44010004</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>44010005</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>44010006</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remake the shop panel
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/NpcShop.xlsx
+++ b/ConfigData/Xlsx/NpcShop.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
-    <sheet name="NpcShop" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -55,10 +55,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>zymu1;zymu2</t>
+    <t>Ename</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>zymu1;zymu2</t>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdaolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zzwandou;zzyumi;zzpingguo;zzlanmei</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -246,7 +259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,8 +445,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -548,6 +567,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -677,14 +727,32 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -732,7 +800,181 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -746,14 +988,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="SellTable"/>
-    <tableColumn id="3" name="MoneyType"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:D4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="6">
+  <autoFilter ref="A3:D4"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="Ename" dataDxfId="4"/>
+    <tableColumn id="3" name="SellTable" dataDxfId="3"/>
+    <tableColumn id="4" name="MoneyType" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1078,134 +1321,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="81.875" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
+    <row r="1" spans="1:4" ht="55.5" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="4">
         <v>44000001</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>44000002</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>44010001</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>44010003</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>44010004</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>44010005</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>44010006</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish one product shop
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/NpcShop.xlsx
+++ b/ConfigData/Xlsx/NpcShop.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -36,68 +36,88 @@
     <t>Id</t>
   </si>
   <si>
+    <t>MoneyType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>货币类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ename</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdaolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zzwandou;zzyumi;zzpingguo;zzlanmei</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sddyeseller</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ranliaohong;ranliaobai;ranliaolv;ranliaohuang;ranliaolan;ranliaozong;ranliaozi;ranliaohei</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RandomChooseX</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机选取</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机道具列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SellRandomTable</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>SellTable</t>
-  </si>
-  <si>
-    <t>MoneyType</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>货币类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ename</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>英文名</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sdaolai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zzwandou;zzyumi;zzpingguo;zzlanmei</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sddyeseller</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ranliaohong;ranliaobai;ranliaolv;ranliaohuang;ranliaolan;ranliaozong;ranliaozi;ranliaohei</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RandomChooseX</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机选取</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdtatamu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spyan;sptang;spmianfen;spcha;spdounai;spniunai;spganlanyou;sphujiaofen;spyumibing;spzhenzhu</t>
+  </si>
+  <si>
+    <t>spputaojiu</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -762,17 +782,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -819,7 +839,36 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1036,14 +1085,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:E5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A3:E5"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Id" dataDxfId="4"/>
-    <tableColumn id="2" name="Ename" dataDxfId="3"/>
-    <tableColumn id="3" name="SellTable" dataDxfId="2"/>
-    <tableColumn id="5" name="RandomChooseX" dataDxfId="1"/>
-    <tableColumn id="4" name="MoneyType" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:F6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A3:F6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ename" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SellTable" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{4BDC02B0-1CDE-45CB-99F6-35D06B2FE67A}" name="SellRandomTable" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="RandomChooseX" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MoneyType" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1369,102 +1419,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.375" customWidth="1"/>
-    <col min="4" max="5" width="6.25" customWidth="1"/>
+    <col min="3" max="3" width="41.125" customWidth="1"/>
+    <col min="4" max="4" width="53.375" customWidth="1"/>
+    <col min="5" max="6" width="6.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="55.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>44000001</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="4">
         <v>0</v>
       </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>44000002</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="4">
+        <v>44000003</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
a random priced shop item implement
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/NpcShop.xlsx
+++ b/ConfigData/Xlsx/NpcShop.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -111,13 +111,29 @@
   </si>
   <si>
     <t>spputaojiu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>价格随机化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RandomPrice</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -766,7 +782,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -793,6 +809,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -839,7 +861,37 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1073,6 +1125,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1085,15 +1205,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:F6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:F6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ename" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SellTable" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{4BDC02B0-1CDE-45CB-99F6-35D06B2FE67A}" name="SellRandomTable" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="RandomChooseX" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MoneyType" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:G6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A3:G6"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Id" dataDxfId="6"/>
+    <tableColumn id="2" name="Ename" dataDxfId="5"/>
+    <tableColumn id="3" name="SellTable" dataDxfId="4"/>
+    <tableColumn id="6" name="SellRandomTable" dataDxfId="3"/>
+    <tableColumn id="5" name="RandomChooseX" dataDxfId="2"/>
+    <tableColumn id="4" name="MoneyType" dataDxfId="1"/>
+    <tableColumn id="7" name="RandomPrice" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1107,7 +1228,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1419,11 +1540,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1432,9 +1553,10 @@
     <col min="3" max="3" width="41.125" customWidth="1"/>
     <col min="4" max="4" width="53.375" customWidth="1"/>
     <col min="5" max="6" width="6.25" customWidth="1"/>
+    <col min="7" max="7" width="5.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1453,8 +1575,11 @@
       <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1473,8 +1598,11 @@
       <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1493,8 +1621,11 @@
       <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>44000001</v>
       </c>
@@ -1511,8 +1642,9 @@
       <c r="F4" s="4">
         <v>0</v>
       </c>
+      <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>44000002</v>
       </c>
@@ -1529,8 +1661,9 @@
       <c r="F5" s="4">
         <v>0</v>
       </c>
+      <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>44000003</v>
       </c>
@@ -1548,13 +1681,17 @@
       </c>
       <c r="F6" s="4">
         <v>0</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add a sell limit for npcshop
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/NpcShop.xlsx
+++ b/ConfigData/Xlsx/NpcShop.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -127,14 +127,22 @@
   </si>
   <si>
     <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>物品数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LimitCount</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +304,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,9 +332,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -782,38 +807,47 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -861,7 +895,36 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1125,74 +1188,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1205,16 +1200,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:G6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A3:G6"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Id" dataDxfId="6"/>
-    <tableColumn id="2" name="Ename" dataDxfId="5"/>
-    <tableColumn id="3" name="SellTable" dataDxfId="4"/>
-    <tableColumn id="6" name="SellRandomTable" dataDxfId="3"/>
-    <tableColumn id="5" name="RandomChooseX" dataDxfId="2"/>
-    <tableColumn id="4" name="MoneyType" dataDxfId="1"/>
-    <tableColumn id="7" name="RandomPrice" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:H6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A3:H6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ename" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SellTable" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="SellRandomTable" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="RandomChooseX" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MoneyType" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="RandomPrice" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{307B16B7-2498-446C-B801-8039B361402E}" name="LimitCount" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1228,7 +1224,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1540,150 +1536,171 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.125" customWidth="1"/>
-    <col min="4" max="4" width="53.375" customWidth="1"/>
-    <col min="5" max="6" width="6.25" customWidth="1"/>
-    <col min="7" max="7" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="4"/>
+    <col min="3" max="3" width="41.125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="53.375" style="4" customWidth="1"/>
+    <col min="5" max="6" width="6.25" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="5.75" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="H2" s="7" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="H3" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
         <v>44000001</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9">
         <v>0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="9">
         <v>0</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="13">
+        <v>99</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
         <v>44000002</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="9">
         <v>3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="9">
         <v>0</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="9">
         <v>44000003</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="9">
         <v>5</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="9">
         <v>0</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="11" t="s">
         <v>27</v>
+      </c>
+      <c r="H6" s="12">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a muyin shop
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/NpcShop.xlsx
+++ b/ConfigData/Xlsx/NpcShop.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -135,6 +135,17 @@
   </si>
   <si>
     <t>LimitCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdmuyin</t>
+  </si>
+  <si>
+    <t>spfenghuangjiang;spganlanyou</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>spyan;spxiangliao;spcha;spdounai;spsichou;spputaojiu</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -807,7 +818,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -848,6 +859,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1200,8 +1214,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:H6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A3:H6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:H7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A3:H7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ename" dataDxfId="6"/>
@@ -1537,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1703,6 +1717,32 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="9">
+        <v>44000004</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="9">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="12">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>